<commit_message>
cleaned up code for Experiences of Racism Deck
</commit_message>
<xml_diff>
--- a/docs/sheddinglight.xlsx
+++ b/docs/sheddinglight.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonetaylor/Documents/mufsdeda/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD050BC5-166F-6044-8E51-61FC3EA80C8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1060" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="1220" yWindow="820" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workbook1.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Workbook1.csv!$A$1:$H$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Workbook1.csv!$A$1:$L$62</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="96">
   <si>
     <t>"Growing up in Larchmont, there have never been many POC surrounding me. Being one of the few and with all of my immediate friends being white, I was often belittled and referred to as the "token black friend." Having these same kids, these friends, ask my permission to use the n-word or excuse them from using it because their favorite (black) artists used it in a song was commonplace, as if it gave them some sort of validation." ~MHS Alumni"#mhs"#blm"#biases"#privilege"#mamaroneck"#larchmont"#mhsalumni</t>
   </si>
@@ -286,12 +292,36 @@
   </si>
   <si>
     <t>verbal, physical, overlooked_by_school, school_denied_opportunity</t>
+  </si>
+  <si>
+    <t>school_officials_involved</t>
+  </si>
+  <si>
+    <t>DASA_mention</t>
+  </si>
+  <si>
+    <t>written_doc</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>mediation</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>verbal, school_denied_opportunity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -946,6 +976,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1270,21 +1308,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="106" workbookViewId="0">
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1301,16 +1338,28 @@
         <v>43</v>
       </c>
       <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1327,16 +1376,28 @@
         <v>2015</v>
       </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" t="s">
         <v>78</v>
       </c>
-      <c r="G2">
+      <c r="K2">
         <v>171</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1353,16 +1414,28 @@
         <v>2014</v>
       </c>
       <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" t="s">
         <v>79</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>88</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1379,16 +1452,28 @@
         <v>2012</v>
       </c>
       <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" t="s">
         <v>80</v>
       </c>
-      <c r="G4">
+      <c r="K4">
         <v>185</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1405,16 +1490,28 @@
         <v>2019</v>
       </c>
       <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" t="s">
         <v>80</v>
       </c>
-      <c r="G5">
-        <v>93</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="K5">
+        <v>93</v>
+      </c>
+      <c r="L5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1431,16 +1528,28 @@
         <v>2019</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6">
+        <v>93</v>
+      </c>
+      <c r="G6" t="s">
         <v>93</v>
       </c>
       <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6">
+        <v>93</v>
+      </c>
+      <c r="L6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1457,16 +1566,28 @@
         <v>2016</v>
       </c>
       <c r="F7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" t="s">
         <v>80</v>
       </c>
-      <c r="G7">
+      <c r="K7">
         <v>152</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1483,16 +1604,28 @@
         <v>2010</v>
       </c>
       <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" t="s">
         <v>79</v>
       </c>
-      <c r="G8">
+      <c r="K8">
         <v>106</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1509,16 +1642,28 @@
         <v>2016</v>
       </c>
       <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" t="s">
         <v>78</v>
       </c>
-      <c r="G9">
+      <c r="K9">
         <v>145</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1535,16 +1680,28 @@
         <v>2015</v>
       </c>
       <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" t="s">
         <v>79</v>
       </c>
-      <c r="G10">
+      <c r="K10">
         <v>148</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1561,16 +1718,28 @@
         <v>2017</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11">
+        <v>93</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11">
         <v>91</v>
       </c>
-      <c r="H11" t="s">
+      <c r="L11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1587,16 +1756,28 @@
         <v>2017</v>
       </c>
       <c r="F12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" t="s">
         <v>80</v>
       </c>
-      <c r="G12">
-        <v>93</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="K12">
+        <v>93</v>
+      </c>
+      <c r="L12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1610,16 +1791,28 @@
         <v>2016</v>
       </c>
       <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" t="s">
         <v>79</v>
       </c>
-      <c r="G13">
+      <c r="K13">
         <v>203</v>
       </c>
-      <c r="H13" t="s">
+      <c r="L13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1636,16 +1829,28 @@
         <v>2013</v>
       </c>
       <c r="F14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" t="s">
         <v>81</v>
       </c>
-      <c r="G14">
+      <c r="K14">
         <v>193</v>
       </c>
-      <c r="H14" t="s">
+      <c r="L14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1662,16 +1867,28 @@
         <v>2013</v>
       </c>
       <c r="F15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" t="s">
         <v>81</v>
       </c>
-      <c r="G15">
+      <c r="K15">
         <v>193</v>
       </c>
-      <c r="H15" t="s">
+      <c r="L15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1688,16 +1905,28 @@
         <v>2014</v>
       </c>
       <c r="F16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" t="s">
         <v>82</v>
       </c>
-      <c r="G16">
+      <c r="K16">
         <v>115</v>
       </c>
-      <c r="H16" t="s">
+      <c r="L16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1714,16 +1943,28 @@
         <v>2016</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17">
+        <v>93</v>
+      </c>
+      <c r="G17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17">
         <v>167</v>
       </c>
-      <c r="H17" t="s">
+      <c r="L17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1740,16 +1981,28 @@
         <v>2020</v>
       </c>
       <c r="F18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="s">
         <v>83</v>
       </c>
-      <c r="G18">
+      <c r="K18">
         <v>81</v>
       </c>
-      <c r="H18" t="s">
+      <c r="L18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1766,16 +2019,28 @@
         <v>2017</v>
       </c>
       <c r="F19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" t="s">
         <v>78</v>
       </c>
-      <c r="G19">
+      <c r="K19">
         <v>176</v>
       </c>
-      <c r="H19" t="s">
+      <c r="L19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1792,16 +2057,28 @@
         <v>2017</v>
       </c>
       <c r="F20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" t="s">
         <v>78</v>
       </c>
-      <c r="G20">
+      <c r="K20">
         <v>176</v>
       </c>
-      <c r="H20" t="s">
+      <c r="L20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1818,16 +2095,28 @@
         <v>2016</v>
       </c>
       <c r="F21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" t="s">
         <v>80</v>
       </c>
-      <c r="G21">
+      <c r="K21">
         <v>167</v>
       </c>
-      <c r="H21" t="s">
+      <c r="L21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1844,16 +2133,28 @@
         <v>2016</v>
       </c>
       <c r="F22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" t="s">
         <v>80</v>
       </c>
-      <c r="G22">
+      <c r="K22">
         <v>167</v>
       </c>
-      <c r="H22" t="s">
+      <c r="L22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1867,16 +2168,28 @@
         <v>51</v>
       </c>
       <c r="F23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" t="s">
         <v>84</v>
       </c>
-      <c r="G23">
+      <c r="K23">
         <v>67</v>
       </c>
-      <c r="H23" t="s">
+      <c r="L23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1893,16 +2206,28 @@
         <v>2021</v>
       </c>
       <c r="F24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" t="s">
+        <v>93</v>
+      </c>
+      <c r="J24" t="s">
         <v>79</v>
       </c>
-      <c r="G24">
+      <c r="K24">
         <v>175</v>
       </c>
-      <c r="H24" t="s">
+      <c r="L24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1919,16 +2244,28 @@
         <v>2016</v>
       </c>
       <c r="F25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" t="s">
         <v>79</v>
       </c>
-      <c r="G25">
+      <c r="K25">
         <v>133</v>
       </c>
-      <c r="H25" t="s">
+      <c r="L25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1942,16 +2279,28 @@
         <v>51</v>
       </c>
       <c r="F26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J26" t="s">
         <v>84</v>
       </c>
-      <c r="G26">
-        <v>93</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="K26">
+        <v>93</v>
+      </c>
+      <c r="L26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1968,16 +2317,28 @@
         <v>2019</v>
       </c>
       <c r="F27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" t="s">
         <v>85</v>
       </c>
-      <c r="G27">
+      <c r="K27">
         <v>118</v>
       </c>
-      <c r="H27" t="s">
+      <c r="L27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1991,16 +2352,28 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
+        <v>93</v>
+      </c>
+      <c r="G28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" t="s">
+        <v>93</v>
+      </c>
+      <c r="J28" t="s">
         <v>83</v>
       </c>
-      <c r="G28">
+      <c r="K28">
         <v>73</v>
       </c>
-      <c r="H28" t="s">
+      <c r="L28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2014,16 +2387,28 @@
         <v>51</v>
       </c>
       <c r="F29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" t="s">
+        <v>93</v>
+      </c>
+      <c r="J29" t="s">
         <v>83</v>
       </c>
-      <c r="G29">
+      <c r="K29">
         <v>147</v>
       </c>
-      <c r="H29" t="s">
+      <c r="L29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2037,16 +2422,28 @@
         <v>48</v>
       </c>
       <c r="F30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" t="s">
+        <v>93</v>
+      </c>
+      <c r="I30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J30" t="s">
         <v>79</v>
       </c>
-      <c r="G30">
+      <c r="K30">
         <v>109</v>
       </c>
-      <c r="H30" t="s">
+      <c r="L30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2060,16 +2457,28 @@
         <v>48</v>
       </c>
       <c r="F31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" t="s">
         <v>80</v>
       </c>
-      <c r="G31">
+      <c r="K31">
         <v>127</v>
       </c>
-      <c r="H31" t="s">
+      <c r="L31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2083,16 +2492,28 @@
         <v>51</v>
       </c>
       <c r="F32" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" t="s">
         <v>80</v>
       </c>
-      <c r="G32">
+      <c r="K32">
         <v>147</v>
       </c>
-      <c r="H32" t="s">
+      <c r="L32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2109,16 +2530,28 @@
         <v>2009</v>
       </c>
       <c r="F33" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" t="s">
         <v>80</v>
       </c>
-      <c r="G33">
+      <c r="K33">
         <v>164</v>
       </c>
-      <c r="H33" t="s">
+      <c r="L33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -2135,16 +2568,28 @@
         <v>2022</v>
       </c>
       <c r="F34" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" t="s">
         <v>79</v>
       </c>
-      <c r="G34">
+      <c r="K34">
         <v>161</v>
       </c>
-      <c r="H34" t="s">
+      <c r="L34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2158,16 +2603,28 @@
         <v>48</v>
       </c>
       <c r="F35" t="s">
-        <v>80</v>
-      </c>
-      <c r="G35">
+        <v>93</v>
+      </c>
+      <c r="G35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" t="s">
+        <v>91</v>
+      </c>
+      <c r="J35" t="s">
+        <v>94</v>
+      </c>
+      <c r="K35">
         <v>150</v>
       </c>
-      <c r="H35" t="s">
+      <c r="L35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2184,16 +2641,28 @@
         <v>2017</v>
       </c>
       <c r="F36" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" t="s">
+        <v>93</v>
+      </c>
+      <c r="I36" t="s">
+        <v>93</v>
+      </c>
+      <c r="J36" t="s">
         <v>79</v>
       </c>
-      <c r="G36">
+      <c r="K36">
         <v>184</v>
       </c>
-      <c r="H36" t="s">
+      <c r="L36" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2207,16 +2676,28 @@
         <v>48</v>
       </c>
       <c r="F37" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" t="s">
+        <v>93</v>
+      </c>
+      <c r="H37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J37" t="s">
         <v>83</v>
       </c>
-      <c r="G37">
+      <c r="K37">
         <v>164</v>
       </c>
-      <c r="H37" t="s">
+      <c r="L37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2230,16 +2711,28 @@
         <v>48</v>
       </c>
       <c r="F38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" t="s">
+        <v>93</v>
+      </c>
+      <c r="I38" t="s">
+        <v>93</v>
+      </c>
+      <c r="J38" t="s">
         <v>83</v>
       </c>
-      <c r="G38">
+      <c r="K38">
         <v>164</v>
       </c>
-      <c r="H38" t="s">
+      <c r="L38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -2253,16 +2746,28 @@
         <v>48</v>
       </c>
       <c r="F39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" t="s">
         <v>81</v>
       </c>
-      <c r="G39">
+      <c r="K39">
         <v>134</v>
       </c>
-      <c r="H39" t="s">
+      <c r="L39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2276,16 +2781,28 @@
         <v>48</v>
       </c>
       <c r="F40" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" t="s">
+        <v>93</v>
+      </c>
+      <c r="H40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40" t="s">
+        <v>93</v>
+      </c>
+      <c r="J40" t="s">
         <v>79</v>
       </c>
-      <c r="G40">
+      <c r="K40">
         <v>61</v>
       </c>
-      <c r="H40" t="s">
+      <c r="L40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2299,16 +2816,28 @@
         <v>48</v>
       </c>
       <c r="F41" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" t="s">
+        <v>93</v>
+      </c>
+      <c r="H41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" t="s">
+        <v>93</v>
+      </c>
+      <c r="J41" t="s">
         <v>86</v>
       </c>
-      <c r="G41">
+      <c r="K41">
         <v>75</v>
       </c>
-      <c r="H41" t="s">
+      <c r="L41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2322,16 +2851,28 @@
         <v>48</v>
       </c>
       <c r="F42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" t="s">
+        <v>93</v>
+      </c>
+      <c r="H42" t="s">
+        <v>93</v>
+      </c>
+      <c r="I42" t="s">
+        <v>93</v>
+      </c>
+      <c r="J42" t="s">
         <v>79</v>
       </c>
-      <c r="G42">
+      <c r="K42">
         <v>91</v>
       </c>
-      <c r="H42" t="s">
+      <c r="L42" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2344,14 +2885,26 @@
       <c r="D43" t="s">
         <v>48</v>
       </c>
-      <c r="G43">
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" t="s">
+        <v>93</v>
+      </c>
+      <c r="H43" t="s">
+        <v>93</v>
+      </c>
+      <c r="I43" t="s">
+        <v>93</v>
+      </c>
+      <c r="K43">
         <v>105</v>
       </c>
-      <c r="H43" t="s">
+      <c r="L43" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2368,16 +2921,28 @@
         <v>2015</v>
       </c>
       <c r="F44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" t="s">
+        <v>93</v>
+      </c>
+      <c r="I44" t="s">
+        <v>93</v>
+      </c>
+      <c r="J44" t="s">
         <v>85</v>
       </c>
-      <c r="G44">
+      <c r="K44">
         <v>139</v>
       </c>
-      <c r="H44" t="s">
+      <c r="L44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2393,14 +2958,26 @@
       <c r="E45">
         <v>2015</v>
       </c>
-      <c r="G45">
+      <c r="F45" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" t="s">
+        <v>93</v>
+      </c>
+      <c r="H45" t="s">
+        <v>93</v>
+      </c>
+      <c r="I45" t="s">
+        <v>93</v>
+      </c>
+      <c r="K45">
         <v>128</v>
       </c>
-      <c r="H45" t="s">
+      <c r="L45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -2417,16 +2994,28 @@
         <v>2017</v>
       </c>
       <c r="F46" t="s">
+        <v>93</v>
+      </c>
+      <c r="G46" t="s">
+        <v>93</v>
+      </c>
+      <c r="H46" t="s">
+        <v>93</v>
+      </c>
+      <c r="I46" t="s">
+        <v>93</v>
+      </c>
+      <c r="J46" t="s">
         <v>79</v>
       </c>
-      <c r="G46">
+      <c r="K46">
         <v>82</v>
       </c>
-      <c r="H46" t="s">
+      <c r="L46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -2443,16 +3032,28 @@
         <v>2014</v>
       </c>
       <c r="F47" t="s">
+        <v>93</v>
+      </c>
+      <c r="G47" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" t="s">
+        <v>93</v>
+      </c>
+      <c r="I47" t="s">
+        <v>93</v>
+      </c>
+      <c r="J47" t="s">
         <v>83</v>
       </c>
-      <c r="G47">
+      <c r="K47">
         <v>88</v>
       </c>
-      <c r="H47" t="s">
+      <c r="L47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -2469,16 +3070,28 @@
         <v>2019</v>
       </c>
       <c r="F48" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" t="s">
+        <v>93</v>
+      </c>
+      <c r="I48" t="s">
+        <v>93</v>
+      </c>
+      <c r="J48" t="s">
         <v>83</v>
       </c>
-      <c r="G48">
+      <c r="K48">
         <v>67</v>
       </c>
-      <c r="H48" t="s">
+      <c r="L48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2492,16 +3105,28 @@
         <v>48</v>
       </c>
       <c r="F49" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" t="s">
+        <v>93</v>
+      </c>
+      <c r="H49" t="s">
+        <v>93</v>
+      </c>
+      <c r="I49" t="s">
+        <v>93</v>
+      </c>
+      <c r="J49" t="s">
         <v>79</v>
       </c>
-      <c r="G49">
+      <c r="K49">
         <v>121</v>
       </c>
-      <c r="H49" t="s">
+      <c r="L49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2518,16 +3143,28 @@
         <v>2014</v>
       </c>
       <c r="F50" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" t="s">
+        <v>93</v>
+      </c>
+      <c r="H50" t="s">
+        <v>93</v>
+      </c>
+      <c r="I50" t="s">
+        <v>93</v>
+      </c>
+      <c r="J50" t="s">
         <v>79</v>
       </c>
-      <c r="G50">
+      <c r="K50">
         <v>106</v>
       </c>
-      <c r="H50" t="s">
+      <c r="L50" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -2541,16 +3178,28 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>81</v>
-      </c>
-      <c r="G51">
+        <v>93</v>
+      </c>
+      <c r="G51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I51" t="s">
+        <v>93</v>
+      </c>
+      <c r="J51" t="s">
+        <v>80</v>
+      </c>
+      <c r="K51">
         <v>104</v>
       </c>
-      <c r="H51" t="s">
+      <c r="L51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2567,16 +3216,28 @@
         <v>2014</v>
       </c>
       <c r="F52" t="s">
-        <v>80</v>
-      </c>
-      <c r="G52">
+        <v>93</v>
+      </c>
+      <c r="G52" t="s">
+        <v>93</v>
+      </c>
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" t="s">
+        <v>93</v>
+      </c>
+      <c r="J52" t="s">
+        <v>79</v>
+      </c>
+      <c r="K52">
         <v>131</v>
       </c>
-      <c r="H52" t="s">
+      <c r="L52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -2590,16 +3251,28 @@
         <v>48</v>
       </c>
       <c r="F53" t="s">
+        <v>91</v>
+      </c>
+      <c r="G53" t="s">
+        <v>93</v>
+      </c>
+      <c r="H53" t="s">
+        <v>93</v>
+      </c>
+      <c r="I53" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" t="s">
         <v>87</v>
       </c>
-      <c r="G53">
+      <c r="K53">
         <v>244</v>
       </c>
-      <c r="H53" t="s">
+      <c r="L53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -2613,16 +3286,28 @@
         <v>48</v>
       </c>
       <c r="F54" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" t="s">
+        <v>93</v>
+      </c>
+      <c r="H54" t="s">
+        <v>93</v>
+      </c>
+      <c r="I54" t="s">
+        <v>93</v>
+      </c>
+      <c r="J54" t="s">
         <v>79</v>
       </c>
-      <c r="G54">
+      <c r="K54">
         <v>164</v>
       </c>
-      <c r="H54" t="s">
+      <c r="L54" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -2636,16 +3321,28 @@
         <v>48</v>
       </c>
       <c r="F55" t="s">
+        <v>93</v>
+      </c>
+      <c r="G55" t="s">
+        <v>93</v>
+      </c>
+      <c r="H55" t="s">
+        <v>93</v>
+      </c>
+      <c r="I55" t="s">
+        <v>95</v>
+      </c>
+      <c r="J55" t="s">
         <v>82</v>
       </c>
-      <c r="G55">
+      <c r="K55">
         <v>245</v>
       </c>
-      <c r="H55" t="s">
+      <c r="L55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -2659,16 +3356,28 @@
         <v>48</v>
       </c>
       <c r="F56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" t="s">
+        <v>93</v>
+      </c>
+      <c r="H56" t="s">
+        <v>93</v>
+      </c>
+      <c r="I56" t="s">
+        <v>95</v>
+      </c>
+      <c r="J56" t="s">
         <v>82</v>
       </c>
-      <c r="G56">
+      <c r="K56">
         <v>245</v>
       </c>
-      <c r="H56" t="s">
+      <c r="L56" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2685,16 +3394,28 @@
         <v>2023</v>
       </c>
       <c r="F57" t="s">
+        <v>93</v>
+      </c>
+      <c r="G57" t="s">
+        <v>93</v>
+      </c>
+      <c r="H57" t="s">
+        <v>93</v>
+      </c>
+      <c r="I57" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" t="s">
         <v>80</v>
       </c>
-      <c r="G57">
+      <c r="K57">
         <v>129</v>
       </c>
-      <c r="H57" t="s">
+      <c r="L57" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -2711,16 +3432,28 @@
         <v>2010</v>
       </c>
       <c r="F58" t="s">
+        <v>93</v>
+      </c>
+      <c r="G58" t="s">
+        <v>93</v>
+      </c>
+      <c r="H58" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" t="s">
         <v>81</v>
       </c>
-      <c r="G58">
+      <c r="K58">
         <v>173</v>
       </c>
-      <c r="H58" t="s">
+      <c r="L58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -2737,16 +3470,28 @@
         <v>2010</v>
       </c>
       <c r="F59" t="s">
+        <v>93</v>
+      </c>
+      <c r="G59" t="s">
+        <v>93</v>
+      </c>
+      <c r="H59" t="s">
+        <v>93</v>
+      </c>
+      <c r="I59" t="s">
+        <v>91</v>
+      </c>
+      <c r="J59" t="s">
         <v>81</v>
       </c>
-      <c r="G59">
+      <c r="K59">
         <v>173</v>
       </c>
-      <c r="H59" t="s">
+      <c r="L59" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>46</v>
       </c>
@@ -2763,16 +3508,28 @@
         <v>2024</v>
       </c>
       <c r="F60" t="s">
+        <v>93</v>
+      </c>
+      <c r="G60" t="s">
+        <v>93</v>
+      </c>
+      <c r="H60" t="s">
+        <v>93</v>
+      </c>
+      <c r="I60" t="s">
+        <v>91</v>
+      </c>
+      <c r="J60" t="s">
         <v>87</v>
       </c>
-      <c r="G60">
+      <c r="K60">
         <v>206</v>
       </c>
-      <c r="H60" t="s">
+      <c r="L60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>47</v>
       </c>
@@ -2789,16 +3546,28 @@
         <v>17</v>
       </c>
       <c r="F61" t="s">
+        <v>93</v>
+      </c>
+      <c r="G61" t="s">
+        <v>93</v>
+      </c>
+      <c r="H61" t="s">
+        <v>93</v>
+      </c>
+      <c r="I61" t="s">
+        <v>91</v>
+      </c>
+      <c r="J61" t="s">
         <v>82</v>
       </c>
-      <c r="G61">
+      <c r="K61">
         <v>193</v>
       </c>
-      <c r="H61" t="s">
+      <c r="L61" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -2812,31 +3581,28 @@
         <v>51</v>
       </c>
       <c r="F62" t="s">
+        <v>93</v>
+      </c>
+      <c r="G62" t="s">
+        <v>93</v>
+      </c>
+      <c r="H62" t="s">
+        <v>93</v>
+      </c>
+      <c r="I62" t="s">
+        <v>93</v>
+      </c>
+      <c r="J62" t="s">
         <v>79</v>
       </c>
-      <c r="G62">
+      <c r="K62">
         <v>83</v>
       </c>
-      <c r="H62" t="s">
+      <c r="L62" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H62">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="school_denied_opportunity"/>
-        <filter val="verbal, internalized, overlooked_by_school"/>
-        <filter val="verbal, overlooked_by_school"/>
-        <filter val="verbal, physical, overlooked_by_school"/>
-        <filter val="verbal, physical, overlooked_by_school, school_denied_opportunity"/>
-        <filter val="verbal,school_denied_opportunity"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:G59">
-      <sortCondition ref="B1:B59"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>